<commit_message>
adding texts file and handling different student ids
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\uni_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF639F-6B0B-465E-96F1-B8A264068972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B181EEA7-46F5-4D0A-8BC7-4FB1B186A1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -114,6 +114,26 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -133,11 +153,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +478,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -468,7 +488,7 @@
     <col min="4" max="4" width="26.625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -490,91 +510,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>